<commit_message>
Cambios VSM, tiempos, cantidades producción, kpi
</commit_message>
<xml_diff>
--- a/Gestion Produccion/GestionProduccion.xlsx
+++ b/Gestion Produccion/GestionProduccion.xlsx
@@ -135,9 +135,6 @@
     <t>Total Tb</t>
   </si>
   <si>
-    <t>Capacidad de producción PC</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>OEE (%)</t>
+  </si>
+  <si>
+    <t>Capacidad de producción (semanal) PC</t>
   </si>
 </sst>
 </file>
@@ -708,15 +708,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -728,15 +719,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -753,6 +735,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1178,7 +1178,7 @@
       <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="42" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -1253,18 +1253,18 @@
   <dimension ref="B1:AB31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="50"/>
     </row>
     <row r="3" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
@@ -1327,17 +1327,17 @@
     </row>
     <row r="7" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="32"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="50"/>
     </row>
     <row r="9" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
@@ -1379,10 +1379,10 @@
         <v>640</v>
       </c>
       <c r="D10" s="29">
-        <v>479</v>
+        <v>339</v>
       </c>
       <c r="E10" s="29">
-        <v>458</v>
+        <v>318</v>
       </c>
       <c r="F10" s="29">
         <v>144</v>
@@ -1399,9 +1399,9 @@
       <c r="J10" s="29">
         <v>20</v>
       </c>
-      <c r="K10" s="34">
+      <c r="K10" s="31">
         <f>SUM(C10:J10)</f>
-        <v>4119</v>
+        <v>3839</v>
       </c>
     </row>
     <row r="11" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1412,10 +1412,10 @@
         <v>640</v>
       </c>
       <c r="D11" s="12">
-        <v>479</v>
+        <v>339</v>
       </c>
       <c r="E11" s="12">
-        <v>458</v>
+        <v>318</v>
       </c>
       <c r="F11" s="12">
         <v>27</v>
@@ -1432,9 +1432,9 @@
       <c r="J11" s="12">
         <v>20</v>
       </c>
-      <c r="K11" s="35">
+      <c r="K11" s="32">
         <f t="shared" ref="K11:K12" si="1">SUM(C11:J11)</f>
-        <v>4132</v>
+        <v>3852</v>
       </c>
     </row>
     <row r="12" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1445,10 +1445,10 @@
         <v>640</v>
       </c>
       <c r="D12" s="15">
-        <v>479</v>
+        <v>339</v>
       </c>
       <c r="E12" s="15">
-        <v>458</v>
+        <v>318</v>
       </c>
       <c r="F12" s="15">
         <v>0</v>
@@ -1465,163 +1465,163 @@
       <c r="J12" s="15">
         <v>20</v>
       </c>
-      <c r="K12" s="36">
+      <c r="K12" s="33">
         <f t="shared" si="1"/>
-        <v>3955</v>
+        <v>3675</v>
       </c>
     </row>
     <row r="13" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="31"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="31"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
-      <c r="X14" s="31"/>
-      <c r="Y14" s="31"/>
-      <c r="Z14" s="31"/>
-      <c r="AA14" s="31"/>
-      <c r="AB14" s="32"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="49"/>
+      <c r="T14" s="49"/>
+      <c r="U14" s="49"/>
+      <c r="V14" s="49"/>
+      <c r="W14" s="49"/>
+      <c r="X14" s="49"/>
+      <c r="Y14" s="49"/>
+      <c r="Z14" s="49"/>
+      <c r="AA14" s="49"/>
+      <c r="AB14" s="50"/>
     </row>
     <row r="15" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="40"/>
-      <c r="C15" s="44" t="s">
+      <c r="B15" s="37"/>
+      <c r="C15" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="44" t="s">
+      <c r="D15" s="52"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="45"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="44" t="s">
+      <c r="G15" s="52"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="45"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="44" t="s">
+      <c r="J15" s="52"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="45"/>
-      <c r="N15" s="46"/>
-      <c r="O15" s="44" t="s">
+      <c r="M15" s="52"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="46"/>
-      <c r="R15" s="44" t="s">
+      <c r="P15" s="52"/>
+      <c r="Q15" s="53"/>
+      <c r="R15" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="S15" s="45"/>
-      <c r="T15" s="46"/>
-      <c r="U15" s="44" t="s">
+      <c r="S15" s="52"/>
+      <c r="T15" s="53"/>
+      <c r="U15" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="V15" s="45"/>
-      <c r="W15" s="46"/>
-      <c r="X15" s="44" t="s">
+      <c r="V15" s="52"/>
+      <c r="W15" s="53"/>
+      <c r="X15" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="Y15" s="45"/>
-      <c r="Z15" s="46"/>
-      <c r="AA15" s="30" t="s">
+      <c r="Y15" s="52"/>
+      <c r="Z15" s="53"/>
+      <c r="AA15" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="AB15" s="32"/>
+      <c r="AB15" s="50"/>
     </row>
     <row r="16" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="F16" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="37" t="s">
+      <c r="G16" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="37" t="s">
+      <c r="H16" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="37" t="s">
+      <c r="I16" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="37" t="s">
+      <c r="J16" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="K16" s="37" t="s">
+      <c r="K16" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="L16" s="37" t="s">
+      <c r="L16" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="M16" s="37" t="s">
+      <c r="M16" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="N16" s="37" t="s">
+      <c r="N16" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="O16" s="37" t="s">
+      <c r="O16" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="P16" s="37" t="s">
+      <c r="P16" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="Q16" s="37" t="s">
+      <c r="Q16" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="R16" s="37" t="s">
+      <c r="R16" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="S16" s="37" t="s">
+      <c r="S16" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="T16" s="37" t="s">
+      <c r="T16" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="U16" s="37" t="s">
+      <c r="U16" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="V16" s="37" t="s">
+      <c r="V16" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="W16" s="37" t="s">
+      <c r="W16" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="X16" s="37" t="s">
+      <c r="X16" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="Y16" s="37" t="s">
+      <c r="Y16" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="Z16" s="37" t="s">
+      <c r="Z16" s="34" t="s">
         <v>37</v>
       </c>
       <c r="AA16" s="6" t="s">
@@ -1635,201 +1635,201 @@
       <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="41">
+      <c r="C17" s="38">
         <v>300</v>
       </c>
-      <c r="D17" s="42">
+      <c r="D17" s="39">
         <f>C17+C10</f>
         <v>940</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E17" s="40">
         <f>3600/D17</f>
         <v>3.8297872340425534</v>
       </c>
-      <c r="F17" s="41">
-        <v>1020</v>
-      </c>
-      <c r="G17" s="42">
+      <c r="F17" s="38">
+        <v>1048</v>
+      </c>
+      <c r="G17" s="39">
         <f>D10+F17</f>
-        <v>1499</v>
-      </c>
-      <c r="H17" s="43">
+        <v>1387</v>
+      </c>
+      <c r="H17" s="40">
         <f>3600/G17</f>
-        <v>2.4016010673782522</v>
-      </c>
-      <c r="I17" s="41">
-        <v>1020</v>
-      </c>
-      <c r="J17" s="42">
+        <v>2.5955299206921412</v>
+      </c>
+      <c r="I17" s="38">
+        <v>1053</v>
+      </c>
+      <c r="J17" s="39">
         <f>I17+E10</f>
-        <v>1478</v>
-      </c>
-      <c r="K17" s="43">
+        <v>1371</v>
+      </c>
+      <c r="K17" s="40">
         <f>3600/J17</f>
-        <v>2.4357239512855209</v>
-      </c>
-      <c r="L17" s="41">
+        <v>2.6258205689277898</v>
+      </c>
+      <c r="L17" s="38">
         <v>30</v>
       </c>
-      <c r="M17" s="42">
+      <c r="M17" s="39">
         <f>L17+F10</f>
         <v>174</v>
       </c>
-      <c r="N17" s="43">
+      <c r="N17" s="40">
         <f>3600/M17</f>
         <v>20.689655172413794</v>
       </c>
-      <c r="O17" s="41">
+      <c r="O17" s="38">
         <v>0</v>
       </c>
-      <c r="P17" s="42">
+      <c r="P17" s="39">
         <f>G10+O17</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="43">
+      <c r="Q17" s="40">
         <v>0</v>
       </c>
-      <c r="R17" s="41">
+      <c r="R17" s="38">
         <v>140</v>
       </c>
-      <c r="S17" s="42">
+      <c r="S17" s="39">
         <f>H10+R17</f>
         <v>2318</v>
       </c>
-      <c r="T17" s="43">
+      <c r="T17" s="40">
         <f>3600/S17</f>
         <v>1.5530629853321829</v>
       </c>
-      <c r="U17" s="41">
+      <c r="U17" s="38">
         <v>75</v>
       </c>
-      <c r="V17" s="42">
+      <c r="V17" s="39">
         <f>I10+U17</f>
         <v>275</v>
       </c>
-      <c r="W17" s="43">
+      <c r="W17" s="40">
         <f>3600/V17</f>
         <v>13.090909090909092</v>
       </c>
-      <c r="X17" s="41">
+      <c r="X17" s="38">
         <v>40</v>
       </c>
-      <c r="Y17" s="42">
+      <c r="Y17" s="39">
         <f>J10+X17</f>
         <v>60</v>
       </c>
-      <c r="Z17" s="43">
+      <c r="Z17" s="40">
         <f>3600/Y17</f>
         <v>60</v>
       </c>
-      <c r="AA17" s="41">
+      <c r="AA17" s="38">
         <f>D17+G17+J17+M17+P17+S17+V17+Y17</f>
-        <v>6744</v>
-      </c>
-      <c r="AB17" s="33">
+        <v>6525</v>
+      </c>
+      <c r="AB17" s="30">
         <f>3600/AA17</f>
-        <v>0.53380782918149461</v>
+        <v>0.55172413793103448</v>
       </c>
     </row>
     <row r="18" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="39">
+      <c r="C18" s="36">
         <v>300</v>
       </c>
       <c r="D18" s="19">
         <f t="shared" ref="D18:D19" si="2">C18+C11</f>
         <v>940</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="32">
         <f t="shared" ref="E18:E19" si="3">3600/D18</f>
         <v>3.8297872340425534</v>
       </c>
-      <c r="F18" s="39">
-        <v>1020</v>
+      <c r="F18" s="36">
+        <v>1048</v>
       </c>
       <c r="G18" s="19">
         <f t="shared" ref="G18:G19" si="4">D11+F18</f>
-        <v>1499</v>
-      </c>
-      <c r="H18" s="35">
+        <v>1387</v>
+      </c>
+      <c r="H18" s="32">
         <f t="shared" ref="H18:H19" si="5">3600/G18</f>
-        <v>2.4016010673782522</v>
-      </c>
-      <c r="I18" s="39">
-        <v>1020</v>
+        <v>2.5955299206921412</v>
+      </c>
+      <c r="I18" s="36">
+        <v>1053</v>
       </c>
       <c r="J18" s="19">
         <f t="shared" ref="J18:J19" si="6">I18+E11</f>
-        <v>1478</v>
-      </c>
-      <c r="K18" s="35">
+        <v>1371</v>
+      </c>
+      <c r="K18" s="32">
         <f t="shared" ref="K18:K19" si="7">3600/J18</f>
-        <v>2.4357239512855209</v>
-      </c>
-      <c r="L18" s="39">
+        <v>2.6258205689277898</v>
+      </c>
+      <c r="L18" s="36">
         <v>30</v>
       </c>
       <c r="M18" s="19">
         <f t="shared" ref="M18:M19" si="8">L18+F11</f>
         <v>57</v>
       </c>
-      <c r="N18" s="35">
-        <f t="shared" ref="N18:N19" si="9">3600/M18</f>
+      <c r="N18" s="32">
+        <f t="shared" ref="N18" si="9">3600/M18</f>
         <v>63.157894736842103</v>
       </c>
-      <c r="O18" s="39">
+      <c r="O18" s="36">
         <v>30</v>
       </c>
       <c r="P18" s="19">
         <f t="shared" ref="P18:P19" si="10">G11+O18</f>
         <v>170</v>
       </c>
-      <c r="Q18" s="35">
-        <f t="shared" ref="Q18:Q19" si="11">3600/P18</f>
+      <c r="Q18" s="32">
+        <f t="shared" ref="Q18" si="11">3600/P18</f>
         <v>21.176470588235293</v>
       </c>
-      <c r="R18" s="39">
+      <c r="R18" s="36">
         <v>140</v>
       </c>
       <c r="S18" s="19">
         <f t="shared" ref="S18:S19" si="12">H11+R18</f>
         <v>2318</v>
       </c>
-      <c r="T18" s="35">
+      <c r="T18" s="32">
         <f t="shared" ref="T18:T19" si="13">3600/S18</f>
         <v>1.5530629853321829</v>
       </c>
-      <c r="U18" s="39">
+      <c r="U18" s="36">
         <v>75</v>
       </c>
       <c r="V18" s="19">
         <f t="shared" ref="V18:V19" si="14">I11+U18</f>
         <v>265</v>
       </c>
-      <c r="W18" s="35">
+      <c r="W18" s="32">
         <f t="shared" ref="W18:W19" si="15">3600/V18</f>
         <v>13.584905660377359</v>
       </c>
-      <c r="X18" s="39">
+      <c r="X18" s="36">
         <v>40</v>
       </c>
       <c r="Y18" s="19">
         <f t="shared" ref="Y18:Y19" si="16">J11+X18</f>
         <v>60</v>
       </c>
-      <c r="Z18" s="35">
+      <c r="Z18" s="32">
         <f t="shared" ref="Z18:Z19" si="17">3600/Y18</f>
         <v>60</v>
       </c>
       <c r="AA18" s="19">
         <f t="shared" ref="AA18:AA19" si="18">D18+G18+J18+M18+P18+S18+V18+Y18</f>
-        <v>6787</v>
-      </c>
-      <c r="AB18" s="47">
+        <v>6568</v>
+      </c>
+      <c r="AB18" s="41">
         <f t="shared" ref="AB18:AB19" si="19">3600/AA18</f>
-        <v>0.53042581405628408</v>
+        <v>0.54811205846528621</v>
       </c>
     </row>
     <row r="19" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1848,26 +1848,26 @@
         <v>3.8297872340425534</v>
       </c>
       <c r="F19" s="9">
-        <v>1020</v>
+        <v>1048</v>
       </c>
       <c r="G19" s="21">
         <f t="shared" si="4"/>
-        <v>1499</v>
+        <v>1387</v>
       </c>
       <c r="H19" s="11">
         <f t="shared" si="5"/>
-        <v>2.4016010673782522</v>
+        <v>2.5955299206921412</v>
       </c>
       <c r="I19" s="9">
-        <v>1020</v>
+        <v>1053</v>
       </c>
       <c r="J19" s="21">
         <f t="shared" si="6"/>
-        <v>1478</v>
+        <v>1371</v>
       </c>
       <c r="K19" s="11">
         <f t="shared" si="7"/>
-        <v>2.4357239512855209</v>
+        <v>2.6258205689277898</v>
       </c>
       <c r="L19" s="9">
         <v>0</v>
@@ -1924,37 +1924,37 @@
       </c>
       <c r="AA19" s="9">
         <f t="shared" si="18"/>
-        <v>6550</v>
+        <v>6331</v>
       </c>
       <c r="AB19" s="21">
         <f t="shared" si="19"/>
-        <v>0.54961832061068705</v>
+        <v>0.56863054809666724</v>
       </c>
     </row>
     <row r="20" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32"/>
+      <c r="C21" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="50"/>
     </row>
     <row r="22" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="34" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="F22" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1963,17 +1963,17 @@
       </c>
       <c r="C23" s="7">
         <f>AB17</f>
-        <v>0.53380782918149461</v>
-      </c>
-      <c r="D23" s="42">
+        <v>0.55172413793103448</v>
+      </c>
+      <c r="D23" s="39">
         <v>5</v>
       </c>
       <c r="E23" s="8">
         <v>7.5</v>
       </c>
-      <c r="F23" s="42">
+      <c r="F23" s="39">
         <f>C23*D23*E23</f>
-        <v>20.017793594306045</v>
+        <v>20.689655172413794</v>
       </c>
     </row>
     <row r="24" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1982,17 +1982,17 @@
       </c>
       <c r="C24" s="19">
         <f t="shared" ref="C24:C25" si="20">AB18</f>
-        <v>0.53042581405628408</v>
+        <v>0.54811205846528621</v>
       </c>
       <c r="D24" s="19">
         <v>5</v>
       </c>
-      <c r="E24" s="35">
+      <c r="E24" s="32">
         <v>7.5</v>
       </c>
       <c r="F24" s="19">
         <f t="shared" ref="F24:F25" si="21">C24*D24*E24</f>
-        <v>19.890968027110652</v>
+        <v>20.554202192448233</v>
       </c>
     </row>
     <row r="25" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2001,7 +2001,7 @@
       </c>
       <c r="C25" s="21">
         <f t="shared" si="20"/>
-        <v>0.54961832061068705</v>
+        <v>0.56863054809666724</v>
       </c>
       <c r="D25" s="21">
         <v>5</v>
@@ -2011,61 +2011,61 @@
       </c>
       <c r="F25" s="21">
         <f t="shared" si="21"/>
-        <v>20.610687022900763</v>
+        <v>21.323645553625024</v>
       </c>
     </row>
     <row r="26" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="50"/>
+    </row>
+    <row r="28" spans="2:28" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="32"/>
-    </row>
-    <row r="28" spans="2:28" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="50" t="s">
+      <c r="D28" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="50" t="s">
+      <c r="E28" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="G28" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="J28" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="K28" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="L28" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="M28" s="43" t="s">
         <v>53</v>
-      </c>
-      <c r="F28" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="G28" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="H28" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="I28" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="J28" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K28" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="L28" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="M28" s="49" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="29" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2075,43 +2075,43 @@
       <c r="C29" s="7">
         <v>6.6159999999999997</v>
       </c>
-      <c r="D29" s="41">
+      <c r="D29" s="38">
         <v>7.5</v>
       </c>
-      <c r="E29" s="42">
+      <c r="E29" s="39">
         <f>C29/D29</f>
         <v>0.88213333333333332</v>
       </c>
       <c r="F29" s="8">
         <v>0.95</v>
       </c>
-      <c r="G29" s="42">
+      <c r="G29" s="39">
         <f>C23*C29</f>
-        <v>3.5316725978647683</v>
-      </c>
-      <c r="H29" s="42">
+        <v>3.6502068965517238</v>
+      </c>
+      <c r="H29" s="39">
         <f>AA17/3600</f>
-        <v>1.8733333333333333</v>
-      </c>
-      <c r="I29" s="42">
+        <v>1.8125</v>
+      </c>
+      <c r="I29" s="39">
         <f>K10/3600</f>
-        <v>1.1441666666666668</v>
-      </c>
-      <c r="J29" s="42">
+        <v>1.0663888888888888</v>
+      </c>
+      <c r="J29" s="39">
         <f>G29*H29/C29</f>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="K29" s="42">
+        <v>1</v>
+      </c>
+      <c r="K29" s="39">
         <f>I29/H29</f>
-        <v>0.61076512455516019</v>
-      </c>
-      <c r="L29" s="42">
+        <v>0.58835249042145588</v>
+      </c>
+      <c r="L29" s="39">
         <f>J29*K29</f>
-        <v>0.61076512455516008</v>
-      </c>
-      <c r="M29" s="42">
+        <v>0.58835249042145588</v>
+      </c>
+      <c r="M29" s="39">
         <f>E29*F29*L29*100</f>
-        <v>51.183746144721219</v>
+        <v>49.305507637292457</v>
       </c>
     </row>
     <row r="30" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2121,27 +2121,27 @@
       <c r="C30" s="19">
         <v>6.6159999999999997</v>
       </c>
-      <c r="D30" s="39">
+      <c r="D30" s="36">
         <v>7.5</v>
       </c>
       <c r="E30" s="19">
         <f t="shared" ref="E30:E31" si="22">C30/D30</f>
         <v>0.88213333333333332</v>
       </c>
-      <c r="F30" s="38">
+      <c r="F30" s="35">
         <v>0.95</v>
       </c>
       <c r="G30" s="19">
         <f t="shared" ref="G30:G31" si="23">C24*C30</f>
-        <v>3.5092971857963753</v>
+        <v>3.6263093788063334</v>
       </c>
       <c r="H30" s="19">
         <f t="shared" ref="H30:H31" si="24">AA18/3600</f>
-        <v>1.8852777777777778</v>
+        <v>1.8244444444444445</v>
       </c>
       <c r="I30" s="19">
         <f t="shared" ref="I30:I31" si="25">K11/3600</f>
-        <v>1.1477777777777778</v>
+        <v>1.07</v>
       </c>
       <c r="J30" s="19">
         <f t="shared" ref="J30:J31" si="26">G30*H30/C30</f>
@@ -2149,15 +2149,15 @@
       </c>
       <c r="K30" s="19">
         <f t="shared" ref="K30:K31" si="27">I30/H30</f>
-        <v>0.60881096213349051</v>
+        <v>0.58647990255785631</v>
       </c>
       <c r="L30" s="19">
         <f t="shared" ref="L30:L31" si="28">J30*K30</f>
-        <v>0.60881096213349051</v>
+        <v>0.58647990255785631</v>
       </c>
       <c r="M30" s="19">
         <f>E30*F30*L30*100</f>
-        <v>51.019982122685526</v>
+        <v>49.148579780755178</v>
       </c>
     </row>
     <row r="31" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2179,49 +2179,49 @@
       </c>
       <c r="G31" s="21">
         <f t="shared" si="23"/>
-        <v>3.7280610687022904</v>
+        <v>3.8570210077396943</v>
       </c>
       <c r="H31" s="21">
         <f t="shared" si="24"/>
-        <v>1.8194444444444444</v>
+        <v>1.7586111111111111</v>
       </c>
       <c r="I31" s="21">
         <f t="shared" si="25"/>
-        <v>1.0986111111111112</v>
+        <v>1.0208333333333333</v>
       </c>
       <c r="J31" s="21">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="K31" s="21">
         <f t="shared" si="27"/>
-        <v>0.60381679389312981</v>
+        <v>0.580477017848681</v>
       </c>
       <c r="L31" s="21">
         <f t="shared" si="28"/>
-        <v>0.60381679389312981</v>
+        <v>0.58047701784868111</v>
       </c>
       <c r="M31" s="21">
         <f>E31*F31*L31*100</f>
-        <v>51.878731297709933</v>
+        <v>49.873424419522991</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C14:AB14"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="C8:K8"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C27:M27"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="L15:N15"/>
-    <mergeCell ref="O15:Q15"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="U15:W15"/>
-    <mergeCell ref="X15:Z15"/>
-    <mergeCell ref="C8:K8"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C14:AB14"/>
-    <mergeCell ref="AA15:AB15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Trabajo en gestión de producción
</commit_message>
<xml_diff>
--- a/Gestion Produccion/GestionProduccion.xlsx
+++ b/Gestion Produccion/GestionProduccion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="55">
   <si>
     <t>Producto</t>
   </si>
@@ -238,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -669,11 +669,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -754,6 +795,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1250,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AB31"/>
+  <dimension ref="B1:AB37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1288,11 +1332,11 @@
         <v>27000</v>
       </c>
       <c r="D4" s="17">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E4" s="18">
         <f>C4/D4</f>
-        <v>675</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="5" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1303,11 +1347,11 @@
         <v>27000</v>
       </c>
       <c r="D5" s="12">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E5" s="18">
         <f t="shared" ref="E5:E6" si="0">C5/D5</f>
-        <v>675</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1318,11 +1362,11 @@
         <v>27000</v>
       </c>
       <c r="D6" s="15">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E6" s="25">
         <f t="shared" si="0"/>
-        <v>675</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="7" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -2206,8 +2250,79 @@
         <v>49.873424419522991</v>
       </c>
     </row>
+    <row r="33" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="54">
+        <f>C23</f>
+        <v>0.55172413793103448</v>
+      </c>
+      <c r="D35" s="30">
+        <f>F23</f>
+        <v>20.689655172413794</v>
+      </c>
+      <c r="E35" s="31">
+        <f>M29</f>
+        <v>49.305507637292457</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="36">
+        <f t="shared" ref="C36:C37" si="29">C24</f>
+        <v>0.54811205846528621</v>
+      </c>
+      <c r="D36" s="19">
+        <f t="shared" ref="D36:D37" si="30">F24</f>
+        <v>20.554202192448233</v>
+      </c>
+      <c r="E36" s="32">
+        <f t="shared" ref="E36:E37" si="31">M30</f>
+        <v>49.148579780755178</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="55">
+        <f t="shared" si="29"/>
+        <v>0.56863054809666724</v>
+      </c>
+      <c r="D37" s="56">
+        <f t="shared" si="30"/>
+        <v>21.323645553625024</v>
+      </c>
+      <c r="E37" s="33">
+        <f t="shared" si="31"/>
+        <v>49.873424419522991</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C27:M27"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="L15:N15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C14:AB14"/>
@@ -2217,11 +2332,6 @@
     <mergeCell ref="U15:W15"/>
     <mergeCell ref="X15:Z15"/>
     <mergeCell ref="C8:K8"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C27:M27"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="L15:N15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>